<commit_message>
Performance evaluation part is updated
finalized
</commit_message>
<xml_diff>
--- a/performance analyze/data collection.xlsx
+++ b/performance analyze/data collection.xlsx
@@ -197,6 +197,33 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$4:$I$9</c:f>
@@ -236,20 +263,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133114880"/>
-        <c:axId val="134415488"/>
+        <c:axId val="215205376"/>
+        <c:axId val="215206912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133114880"/>
+        <c:axId val="215205376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134415488"/>
+        <c:crossAx val="215206912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -257,7 +285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134415488"/>
+        <c:axId val="215206912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133114880"/>
+        <c:crossAx val="215205376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -311,6 +339,27 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$11:$I$14</c:f>
@@ -344,20 +393,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133151744"/>
-        <c:axId val="134431488"/>
+        <c:axId val="216221952"/>
+        <c:axId val="216223744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133151744"/>
+        <c:axId val="216221952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134431488"/>
+        <c:crossAx val="216223744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -365,7 +415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134431488"/>
+        <c:axId val="216223744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133151744"/>
+        <c:crossAx val="216221952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -479,11 +529,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135507968"/>
-        <c:axId val="135509504"/>
+        <c:axId val="216230912"/>
+        <c:axId val="216257280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135507968"/>
+        <c:axId val="216230912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,7 +543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135509504"/>
+        <c:crossAx val="216257280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -501,7 +551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135509504"/>
+        <c:axId val="216257280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135507968"/>
+        <c:crossAx val="216230912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -609,11 +659,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135500160"/>
-        <c:axId val="135501696"/>
+        <c:axId val="216604672"/>
+        <c:axId val="216606208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135500160"/>
+        <c:axId val="216604672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,7 +673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135501696"/>
+        <c:crossAx val="216606208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -631,7 +681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135501696"/>
+        <c:axId val="216606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135500160"/>
+        <c:crossAx val="216604672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,15 +714,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>384369</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -694,15 +744,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>15046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1171,7 +1221,7 @@
         <v>5000</v>
       </c>
       <c r="I4">
-        <f>H4*1000/G4</f>
+        <f t="shared" ref="I4:I9" si="0">H4*1000/G4</f>
         <v>32.810767181358237</v>
       </c>
       <c r="J4" s="1">
@@ -1201,7 +1251,7 @@
         <v>5000</v>
       </c>
       <c r="I5">
-        <f>H5*1000/G5</f>
+        <f t="shared" si="0"/>
         <v>45.499217413460485</v>
       </c>
       <c r="J5" s="1">
@@ -1231,7 +1281,7 @@
         <v>5000</v>
       </c>
       <c r="I6" s="2">
-        <f>H6*1000/G6</f>
+        <f t="shared" si="0"/>
         <v>55.030321707260704</v>
       </c>
     </row>
@@ -1258,7 +1308,7 @@
         <v>5000</v>
       </c>
       <c r="I7" s="3">
-        <f>H7*1000/G7</f>
+        <f t="shared" si="0"/>
         <v>54.510171598020193</v>
       </c>
       <c r="J7" s="1">
@@ -1288,7 +1338,7 @@
         <v>5000</v>
       </c>
       <c r="I8" s="3">
-        <f>H8*1000/G8</f>
+        <f t="shared" si="0"/>
         <v>53.400546821599455</v>
       </c>
       <c r="J8" s="1">
@@ -1318,7 +1368,7 @@
         <v>5000</v>
       </c>
       <c r="I9" s="3">
-        <f>H9*1000/G9</f>
+        <f t="shared" si="0"/>
         <v>50.716625924310506</v>
       </c>
       <c r="J9" s="1">

</xml_diff>